<commit_message>
several new people added
</commit_message>
<xml_diff>
--- a/images/images_sizing(AutoRecovered).xlsx
+++ b/images/images_sizing(AutoRecovered).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nitra/git/slovenskivedci/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61B2D9D5-95AA-4340-B32A-A5B40DF02182}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEE99B02-51E4-A346-9F86-8C4EA008BDE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="140" yWindow="500" windowWidth="26740" windowHeight="15460" xr2:uid="{FBABA11E-B330-2F49-B6C1-0584A0817DCB}"/>
+    <workbookView xWindow="13840" yWindow="500" windowWidth="13040" windowHeight="15460" xr2:uid="{FBABA11E-B330-2F49-B6C1-0584A0817DCB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -409,11 +409,11 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>420</v>
+        <v>1000</v>
       </c>
       <c r="B2">
         <f>$B$1/$A$1*A2</f>
-        <v>235.92187500000003</v>
+        <v>561.71875</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new person: Miroslava Kacaniova
</commit_message>
<xml_diff>
--- a/images/images_sizing(AutoRecovered).xlsx
+++ b/images/images_sizing(AutoRecovered).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nitra/git/slovenskivedci/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E7D49B5-2DE8-FA4A-A8A4-AF92BB5BDCFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEDB2281-45FB-9544-9BBD-B5C0EC38DB79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1760" yWindow="500" windowWidth="25320" windowHeight="14880" xr2:uid="{FBABA11E-B330-2F49-B6C1-0584A0817DCB}"/>
+    <workbookView xWindow="1560" yWindow="500" windowWidth="25320" windowHeight="14880" xr2:uid="{FBABA11E-B330-2F49-B6C1-0584A0817DCB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -476,10 +476,10 @@
     <row r="3" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <f>B3/B1*A1</f>
-        <v>534.07510431154378</v>
+        <v>1958.2753824756605</v>
       </c>
       <c r="B3" s="4">
-        <v>300</v>
+        <v>1100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>